<commit_message>
AFL single engine aggregate, apply, etc.
</commit_message>
<xml_diff>
--- a/src/main/resources/tpch_queries/TPCH times.xlsx
+++ b/src/main/resources/tpch_queries/TPCH times.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jack/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Jack/jworkspace/BigDAWGMiddleWare/bigdawgmiddle/src/main/resources/tpch_queries/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
   <si>
     <t>TPCH query number (Postgres)</t>
   </si>
@@ -37,15 +37,58 @@
   <si>
     <t>Average</t>
   </si>
+  <si>
+    <t>TPCH query number (SciDB)</t>
+  </si>
+  <si>
+    <t>&gt;2h</t>
+  </si>
+  <si>
+    <t>??</t>
+  </si>
+  <si>
+    <t>dim</t>
+  </si>
+  <si>
+    <t>&gt; 1h</t>
+  </si>
+  <si>
+    <t>Postgres</t>
+  </si>
+  <si>
+    <t>SciDB</t>
+  </si>
+  <si>
+    <t>&gt; 91 mins</t>
+  </si>
+  <si>
+    <t>&gt; 80 mins</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -68,8 +111,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -80,7 +127,11 @@
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -91,6 +142,2110 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400"/>
+              <a:t>TPCH</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" sz="2400" baseline="0"/>
+              <a:t> query run-time comparison</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US" sz="2400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Postgres</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$40:$M$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$41:$M$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>14436.56928</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>359.80276</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2388.75144</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1562.39528</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1536.11064</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>340.1295200000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2304.15056</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1513.8584</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1527.48504</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5131.2058</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SciDB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$40:$M$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$42:$M$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="10"/>
+                <c:pt idx="0">
+                  <c:v>155403.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45758.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74437.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>52958.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22827.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12128.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90347.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>169667.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22251.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>70561.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-2087180672"/>
+        <c:axId val="-2087467616"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2087180672"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="2000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2087467616"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2087467616"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2087180672"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+        <c:dispUnits>
+          <c:builtInUnit val="thousands"/>
+        </c:dispUnits>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$41</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Postgres</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$40:$N$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$41:$N$41</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>14436.56928</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>359.80276</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2388.75144</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1562.39528</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1536.11064</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>340.1295200000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2304.15056</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1513.8584</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1527.48504</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>5131.2058</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>3749.06448</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$C$42</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>SciDB</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$D$40:$N$40</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>1.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>14.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>18.0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$D$42:$N$42</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="11"/>
+                <c:pt idx="0">
+                  <c:v>155403.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>45758.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>74437.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>52958.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>22827.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>12128.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>90347.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>169667.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>22251.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>70561.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.444197E6</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="-2082806880"/>
+        <c:axId val="-2082587600"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="-2082806880"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2082587600"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="-2082587600"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="-2082806880"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>241300</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>15</xdr:col>
+      <xdr:colOff>419100</xdr:colOff>
+      <xdr:row>69</xdr:row>
+      <xdr:rowOff>177800</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>254000</xdr:colOff>
+      <xdr:row>25</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>698500</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>88900</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="6" name="Chart 5"/>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -356,10 +2511,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Q28"/>
+  <dimension ref="A1:Q42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q28" sqref="Q28"/>
+    <sheetView tabSelected="1" topLeftCell="A20" workbookViewId="0">
+      <selection activeCell="O42" sqref="O42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1855,10 +4010,396 @@
         <v>3749.0644799999995</v>
       </c>
     </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="B30" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
+      <c r="H30" s="2"/>
+      <c r="I30" s="2"/>
+      <c r="J30" s="2"/>
+      <c r="K30" s="2"/>
+      <c r="L30" s="2"/>
+      <c r="M30" s="2"/>
+      <c r="N30" s="2"/>
+      <c r="O30" s="2"/>
+      <c r="P30" s="2"/>
+      <c r="Q30" s="2"/>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A31" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B31">
+        <v>1</v>
+      </c>
+      <c r="C31">
+        <v>2</v>
+      </c>
+      <c r="D31">
+        <v>3</v>
+      </c>
+      <c r="E31">
+        <v>4</v>
+      </c>
+      <c r="F31">
+        <v>5</v>
+      </c>
+      <c r="G31">
+        <v>6</v>
+      </c>
+      <c r="H31">
+        <v>7</v>
+      </c>
+      <c r="I31">
+        <v>8</v>
+      </c>
+      <c r="J31">
+        <v>9</v>
+      </c>
+      <c r="K31">
+        <v>10</v>
+      </c>
+      <c r="L31">
+        <v>11</v>
+      </c>
+      <c r="M31">
+        <v>12</v>
+      </c>
+      <c r="N31">
+        <v>14</v>
+      </c>
+      <c r="O31">
+        <v>15</v>
+      </c>
+      <c r="P31">
+        <v>16</v>
+      </c>
+      <c r="Q31">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.2">
+      <c r="A32">
+        <v>1</v>
+      </c>
+      <c r="B32" s="1">
+        <v>155403</v>
+      </c>
+      <c r="C32" s="1">
+        <v>45758</v>
+      </c>
+      <c r="D32" s="1">
+        <v>74437</v>
+      </c>
+      <c r="E32" s="1">
+        <v>52958</v>
+      </c>
+      <c r="F32" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32" s="1">
+        <v>22827</v>
+      </c>
+      <c r="H32" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+      <c r="K32" s="1"/>
+      <c r="L32" s="1">
+        <v>12128</v>
+      </c>
+      <c r="M32" s="1">
+        <v>90347</v>
+      </c>
+      <c r="N32" s="1">
+        <v>169667</v>
+      </c>
+      <c r="O32" s="1">
+        <v>22251</v>
+      </c>
+      <c r="P32" s="1">
+        <v>70561</v>
+      </c>
+      <c r="Q32" s="1">
+        <v>1444197</v>
+      </c>
+    </row>
+    <row r="36" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B36">
+        <v>1</v>
+      </c>
+      <c r="C36">
+        <v>2</v>
+      </c>
+      <c r="D36">
+        <v>3</v>
+      </c>
+      <c r="E36">
+        <v>4</v>
+      </c>
+      <c r="F36">
+        <v>5</v>
+      </c>
+      <c r="G36">
+        <v>6</v>
+      </c>
+      <c r="H36">
+        <v>7</v>
+      </c>
+      <c r="I36">
+        <v>8</v>
+      </c>
+      <c r="J36">
+        <v>9</v>
+      </c>
+      <c r="K36">
+        <v>10</v>
+      </c>
+      <c r="L36">
+        <v>11</v>
+      </c>
+      <c r="M36">
+        <v>12</v>
+      </c>
+      <c r="N36">
+        <v>14</v>
+      </c>
+      <c r="O36">
+        <v>15</v>
+      </c>
+      <c r="P36">
+        <v>16</v>
+      </c>
+      <c r="Q36">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="37" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B37">
+        <v>14436.569279999998</v>
+      </c>
+      <c r="C37">
+        <v>359.80275999999998</v>
+      </c>
+      <c r="D37">
+        <v>2388.7514399999995</v>
+      </c>
+      <c r="E37">
+        <v>1562.39528</v>
+      </c>
+      <c r="F37">
+        <v>746.50243999999986</v>
+      </c>
+      <c r="G37">
+        <v>1536.1106399999999</v>
+      </c>
+      <c r="H37">
+        <v>1648.37832</v>
+      </c>
+      <c r="I37">
+        <v>2082.76244</v>
+      </c>
+      <c r="J37">
+        <v>6035.0250800000003</v>
+      </c>
+      <c r="K37">
+        <v>1737.2047599999999</v>
+      </c>
+      <c r="L37">
+        <v>340.12952000000007</v>
+      </c>
+      <c r="M37">
+        <v>2304.15056</v>
+      </c>
+      <c r="N37">
+        <v>1513.8584000000001</v>
+      </c>
+      <c r="O37">
+        <v>1527.4850400000003</v>
+      </c>
+      <c r="P37">
+        <v>5131.2057999999997</v>
+      </c>
+      <c r="Q37">
+        <v>3749.0644799999995</v>
+      </c>
+    </row>
+    <row r="38" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="B38">
+        <v>155403</v>
+      </c>
+      <c r="C38">
+        <v>45758</v>
+      </c>
+      <c r="D38">
+        <v>74437</v>
+      </c>
+      <c r="E38">
+        <v>52958</v>
+      </c>
+      <c r="F38" t="s">
+        <v>7</v>
+      </c>
+      <c r="G38">
+        <v>22827</v>
+      </c>
+      <c r="H38" t="s">
+        <v>10</v>
+      </c>
+      <c r="J38" t="s">
+        <v>11</v>
+      </c>
+      <c r="K38" t="s">
+        <v>6</v>
+      </c>
+      <c r="L38">
+        <v>12128</v>
+      </c>
+      <c r="M38">
+        <v>90347</v>
+      </c>
+      <c r="N38">
+        <v>169667</v>
+      </c>
+      <c r="O38">
+        <v>22251</v>
+      </c>
+      <c r="P38">
+        <v>70561</v>
+      </c>
+      <c r="Q38">
+        <v>1444197</v>
+      </c>
+    </row>
+    <row r="39" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="Q39">
+        <v>1147295</v>
+      </c>
+    </row>
+    <row r="40" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="D40">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>2</v>
+      </c>
+      <c r="F40">
+        <v>3</v>
+      </c>
+      <c r="G40">
+        <v>4</v>
+      </c>
+      <c r="H40">
+        <v>6</v>
+      </c>
+      <c r="I40">
+        <v>11</v>
+      </c>
+      <c r="J40">
+        <v>12</v>
+      </c>
+      <c r="K40">
+        <v>14</v>
+      </c>
+      <c r="L40">
+        <v>15</v>
+      </c>
+      <c r="M40">
+        <v>16</v>
+      </c>
+      <c r="N40">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="41" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C41" t="s">
+        <v>8</v>
+      </c>
+      <c r="D41">
+        <v>14436.569279999998</v>
+      </c>
+      <c r="E41">
+        <v>359.80275999999998</v>
+      </c>
+      <c r="F41">
+        <v>2388.7514399999995</v>
+      </c>
+      <c r="G41">
+        <v>1562.39528</v>
+      </c>
+      <c r="H41">
+        <v>1536.1106399999999</v>
+      </c>
+      <c r="I41">
+        <v>340.12952000000007</v>
+      </c>
+      <c r="J41">
+        <v>2304.15056</v>
+      </c>
+      <c r="K41">
+        <v>1513.8584000000001</v>
+      </c>
+      <c r="L41">
+        <v>1527.4850400000003</v>
+      </c>
+      <c r="M41">
+        <v>5131.2057999999997</v>
+      </c>
+      <c r="N41">
+        <v>3749.0644799999995</v>
+      </c>
+    </row>
+    <row r="42" spans="2:17" x14ac:dyDescent="0.2">
+      <c r="C42" t="s">
+        <v>9</v>
+      </c>
+      <c r="D42">
+        <v>155403</v>
+      </c>
+      <c r="E42">
+        <v>45758</v>
+      </c>
+      <c r="F42">
+        <v>74437</v>
+      </c>
+      <c r="G42">
+        <v>52958</v>
+      </c>
+      <c r="H42">
+        <v>22827</v>
+      </c>
+      <c r="I42">
+        <v>12128</v>
+      </c>
+      <c r="J42">
+        <v>90347</v>
+      </c>
+      <c r="K42">
+        <v>169667</v>
+      </c>
+      <c r="L42">
+        <v>22251</v>
+      </c>
+      <c r="M42">
+        <v>70561</v>
+      </c>
+      <c r="N42">
+        <v>1444197</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="B1:Q1"/>
+    <mergeCell ref="B30:Q30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>